<commit_message>
Update to pythonicaally input data
</commit_message>
<xml_diff>
--- a/prep_and_checklists/Breann Lydon  /PREPLIST_Breann Lydon  _10-16-2025_0.xlsx
+++ b/prep_and_checklists/Breann Lydon  /PREPLIST_Breann Lydon  _10-16-2025_0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davidcuvin/purveyor_project/prep_and_checklists/Breann Lydon  /"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ED54EE5-1DC9-0C47-8462-4DC4FCC50A5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B6E9AA-D157-EA4F-A64A-1D6A1D26AD6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -859,10 +859,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="104" workbookViewId="0">
+      <selection activeCell="H53" sqref="H53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1258,8 +1261,8 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="73" orientation="portrait"/>
 </worksheet>
 </file>
 
@@ -1681,5 +1684,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>